<commit_message>
book texture & mapping 1
</commit_message>
<xml_diff>
--- a/ghostTypesAndEvidences.xlsx
+++ b/ghostTypesAndEvidences.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\kantorphobia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0AEDD6-3B73-43D6-B6A8-7C6D2A6FE9DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DB531A-E0F8-4CE9-BA6A-B9DCBD7F84DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6B5883DE-739C-4214-AD19-23CB3CB71906}"/>
+    <workbookView xWindow="-24600" yWindow="1305" windowWidth="21600" windowHeight="11385" xr2:uid="{6B5883DE-739C-4214-AD19-23CB3CB71906}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="22">
   <si>
     <t>Ghost types &amp; their evidence</t>
   </si>
@@ -78,6 +78,30 @@
   </si>
   <si>
     <t>EMF</t>
+  </si>
+  <si>
+    <t>Stejskal</t>
+  </si>
+  <si>
+    <t>Bakalari</t>
+  </si>
+  <si>
+    <t>Code writing</t>
+  </si>
+  <si>
+    <t>Skarka</t>
+  </si>
+  <si>
+    <t>Lazarov</t>
+  </si>
+  <si>
+    <t>Bobek</t>
+  </si>
+  <si>
+    <t>Virtualka</t>
+  </si>
+  <si>
+    <t>Speech</t>
   </si>
 </sst>
 </file>
@@ -433,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC79C332-B304-41ED-A9AB-62AB31DA5B11}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,6 +579,67 @@
         <v>11</v>
       </c>
     </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>

</xml_diff>